<commit_message>
make kinor changes pass and con_pass
</commit_message>
<xml_diff>
--- a/src/test/resources/resources/OrangeHRM.xlsx
+++ b/src/test/resources/resources/OrangeHRM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\git\Orange-HRM\src\test\resources\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC4392F-A21F-4383-AD69-5FB81D23169C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B048DD-A4B2-469E-9CAC-28EBF0FA320E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{18648C37-AC70-4A24-9965-AA15281F9F42}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>serial no</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Rocky</t>
   </si>
   <si>
-    <t>Rocky@123</t>
-  </si>
-  <si>
     <t>Serial no</t>
   </si>
   <si>
@@ -75,10 +72,7 @@
     <t>Pandita</t>
   </si>
   <si>
-    <t>Anil123</t>
-  </si>
-  <si>
-    <t>Ajay123</t>
+    <t>Rocky123</t>
   </si>
 </sst>
 </file>
@@ -518,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -527,7 +521,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -550,16 +544,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -567,16 +561,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -584,16 +578,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -601,7 +595,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{3C40DCEE-39E5-4DF2-A160-1D63706084BE}"/>
+    <hyperlink ref="C3" r:id="rId1" display="Rocky@123" xr:uid="{3C40DCEE-39E5-4DF2-A160-1D63706084BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>